<commit_message>
Horashim Event files update
</commit_message>
<xml_diff>
--- a/events/Horashim_2022/StartList.xlsx
+++ b/events/Horashim_2022/StartList.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106">
   <si>
     <t>STNO</t>
   </si>
@@ -16,52 +16,106 @@
     <t>NAME</t>
   </si>
   <si>
+    <t>מורג בועז</t>
+  </si>
+  <si>
+    <t>זיינפלד עופר</t>
+  </si>
+  <si>
+    <t>מינסקי מנחם</t>
+  </si>
+  <si>
+    <t>סופר עופר</t>
+  </si>
+  <si>
     <t>הימן יונה</t>
   </si>
   <si>
+    <t>דודלזק צביקה</t>
+  </si>
+  <si>
+    <t>וולשטיין דן</t>
+  </si>
+  <si>
+    <t>אשל סהר</t>
+  </si>
+  <si>
+    <t>אשל חגי</t>
+  </si>
+  <si>
+    <t>פלוטקין רון</t>
+  </si>
+  <si>
+    <t>הימן רפי</t>
+  </si>
+  <si>
+    <t>לדרר חגי</t>
+  </si>
+  <si>
+    <t>רימרמן-שדמה נטע</t>
+  </si>
+  <si>
+    <t>ליפוביץ אלכס</t>
+  </si>
+  <si>
+    <t>גולדנר יקיר</t>
+  </si>
+  <si>
+    <t>מלץ אבי</t>
+  </si>
+  <si>
+    <t>אלוש רות</t>
+  </si>
+  <si>
+    <t>פרידמן אלכס</t>
+  </si>
+  <si>
+    <t>מאירי נעם</t>
+  </si>
+  <si>
     <t>צ'רני הלל</t>
   </si>
   <si>
-    <t>מאירי נעם</t>
-  </si>
-  <si>
-    <t>פרידמן אלכס</t>
-  </si>
-  <si>
-    <t>אלוש רות</t>
-  </si>
-  <si>
-    <t>מלץ אבי</t>
-  </si>
-  <si>
-    <t>גולדנר יקיר</t>
-  </si>
-  <si>
-    <t>ליפוביץ אלכס</t>
-  </si>
-  <si>
-    <t>רימרמן-שדמה נטע</t>
-  </si>
-  <si>
-    <t>מורג בועז</t>
-  </si>
-  <si>
-    <t>הימן רפי</t>
-  </si>
-  <si>
     <t>צפורי דרור</t>
   </si>
   <si>
-    <t>אשל חגי</t>
-  </si>
-  <si>
-    <t>אשל סהר</t>
-  </si>
-  <si>
-    <t>פלוטקין רון</t>
-  </si>
-  <si>
-    <t>לדרר חגי</t>
+    <t>פילו בועז</t>
+  </si>
+  <si>
+    <t>כספי שי</t>
+  </si>
+  <si>
+    <t>טל אביב</t>
+  </si>
+  <si>
+    <t>שפר שחר</t>
+  </si>
+  <si>
+    <t>מסינג ענת סיפורים</t>
+  </si>
+  <si>
+    <t>דביר יונתן</t>
+  </si>
+  <si>
+    <t>איגנטוב אידה</t>
+  </si>
+  <si>
+    <t>איגנטוב אנה</t>
+  </si>
+  <si>
+    <t>איגנטוב אנדרי</t>
+  </si>
+  <si>
+    <t>גולדהכט גיורא</t>
+  </si>
+  <si>
+    <t>יודפת עופר</t>
+  </si>
+  <si>
+    <t>ליבר דן</t>
+  </si>
+  <si>
+    <t>משלי יובל</t>
   </si>
   <si>
     <t>משלי ליסה</t>
@@ -79,52 +133,37 @@
     <t>אורי אופיר</t>
   </si>
   <si>
-    <t>וולשטיין דן</t>
+    <t>פילו שמואליק</t>
   </si>
   <si>
     <t>שפירא אורן</t>
   </si>
   <si>
-    <t>דודלזק צביקה</t>
-  </si>
-  <si>
-    <t>ליבר דן</t>
-  </si>
-  <si>
-    <t>גולדהכט גיורא</t>
-  </si>
-  <si>
-    <t>זיינפלד עופר</t>
-  </si>
-  <si>
-    <t>מינסקי מנחם</t>
-  </si>
-  <si>
-    <t>סופר עופר</t>
-  </si>
-  <si>
-    <t>משלי יובל</t>
-  </si>
-  <si>
-    <t>פילו שמואליק</t>
+    <t>חוחלובה טטיאנה</t>
+  </si>
+  <si>
+    <t>נתיב רות</t>
   </si>
   <si>
     <t>CLUB</t>
   </si>
   <si>
+    <t>עמק חפר</t>
+  </si>
+  <si>
+    <t>חבל מודיעין</t>
+  </si>
+  <si>
     <t>השרון</t>
   </si>
   <si>
-    <t>חבל מודיעין</t>
+    <t>לב השרון-מנשה</t>
   </si>
   <si>
     <t>אסא תל אביב</t>
   </si>
   <si>
-    <t>עמק חפר</t>
-  </si>
-  <si>
-    <t>לב השרון-מנשה</t>
+    <t>ראשון לציון</t>
   </si>
   <si>
     <t>CLASS NAME</t>
@@ -133,12 +172,12 @@
     <t>קצר</t>
   </si>
   <si>
+    <t>בינוני</t>
+  </si>
+  <si>
     <t>ארוך</t>
   </si>
   <si>
-    <t>בינוני</t>
-  </si>
-  <si>
     <t>קצרצר</t>
   </si>
   <si>
@@ -157,12 +196,12 @@
     <t>SEX</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>הערות</t>
   </si>
   <si>
@@ -184,46 +223,91 @@
     <t>נייד</t>
   </si>
   <si>
+    <t>050-4270094</t>
+  </si>
+  <si>
+    <t>050-8800048</t>
+  </si>
+  <si>
+    <t>050-8802248</t>
+  </si>
+  <si>
+    <t>054-3291072</t>
+  </si>
+  <si>
     <t>054-5745695</t>
   </si>
   <si>
+    <t>050-5820593</t>
+  </si>
+  <si>
+    <t>054-3080103</t>
+  </si>
+  <si>
+    <t>054-4683685</t>
+  </si>
+  <si>
+    <t>054-4624616</t>
+  </si>
+  <si>
+    <t>054-7205695</t>
+  </si>
+  <si>
+    <t>058-5657981</t>
+  </si>
+  <si>
+    <t>052-2512440</t>
+  </si>
+  <si>
+    <t>054-5986439</t>
+  </si>
+  <si>
+    <t>054-4225931</t>
+  </si>
+  <si>
+    <t>050-5525774</t>
+  </si>
+  <si>
+    <t>054-4460223</t>
+  </si>
+  <si>
+    <t>050-6220411</t>
+  </si>
+  <si>
     <t>052-3614791</t>
   </si>
   <si>
-    <t>050-6220411</t>
-  </si>
-  <si>
-    <t>054-4460223</t>
-  </si>
-  <si>
-    <t>050-5525774</t>
-  </si>
-  <si>
-    <t>054-4225931</t>
-  </si>
-  <si>
-    <t>054-5986439</t>
-  </si>
-  <si>
-    <t>052-2512440</t>
-  </si>
-  <si>
-    <t>050-4270094</t>
-  </si>
-  <si>
-    <t>054-7205695</t>
-  </si>
-  <si>
     <t>050-4813400</t>
   </si>
   <si>
-    <t>054-4683685</t>
-  </si>
-  <si>
-    <t>054-4624616</t>
-  </si>
-  <si>
-    <t>058-5657981</t>
+    <t>054-7236295</t>
+  </si>
+  <si>
+    <t>054-7864656</t>
+  </si>
+  <si>
+    <t>058-4741993</t>
+  </si>
+  <si>
+    <t>052-6867272</t>
+  </si>
+  <si>
+    <t>054-2344862</t>
+  </si>
+  <si>
+    <t>054-6998499</t>
+  </si>
+  <si>
+    <t>052-5811811</t>
+  </si>
+  <si>
+    <t>052-3351212</t>
+  </si>
+  <si>
+    <t>054-4481312</t>
+  </si>
+  <si>
+    <t>054-4468818</t>
   </si>
   <si>
     <t>054-5390821</t>
@@ -235,31 +319,13 @@
     <t>054-3250080</t>
   </si>
   <si>
-    <t>054-3080103</t>
-  </si>
-  <si>
     <t>054-6697140</t>
   </si>
   <si>
-    <t>050-5820593</t>
-  </si>
-  <si>
-    <t>054-4481312</t>
-  </si>
-  <si>
-    <t>052-5811811</t>
-  </si>
-  <si>
-    <t>050-8800048</t>
-  </si>
-  <si>
-    <t>050-8802248</t>
-  </si>
-  <si>
-    <t>054-3291072</t>
-  </si>
-  <si>
-    <t>054-4468818</t>
+    <t>054-9949571</t>
+  </si>
+  <si>
+    <t>054-4683928</t>
   </si>
 </sst>
 </file>
@@ -422,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView zoomScale="100" topLeftCell="A1" workbookViewId="0" showGridLines="true" showRowColHeaders="true"/>
   </sheetViews>
@@ -436,70 +502,70 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="L1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="N1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3279</v>
+        <v>1465</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="n">
-        <v>2071090</v>
+        <v>2071190</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J2"/>
       <c r="K2" t="b">
@@ -507,38 +573,40 @@
       </c>
       <c r="L2"/>
       <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2"/>
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>69</v>
+      </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2029</v>
+        <v>6283</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="n">
-        <v>2071030</v>
+        <v>2071517</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J3"/>
       <c r="K3" t="b">
@@ -546,38 +614,38 @@
       </c>
       <c r="L3"/>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N3"/>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3734</v>
+        <v>603</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" t="n">
-        <v>2071186</v>
+        <v>2071005</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J4"/>
       <c r="K4" t="b">
@@ -585,38 +653,38 @@
       </c>
       <c r="L4"/>
       <c r="M4" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N4"/>
       <c r="O4" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2599</v>
+        <v>7207</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0.395833333333333</v>
+        <v>0.375</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" t="n">
-        <v>230740</v>
+        <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J5"/>
       <c r="K5" t="b">
@@ -624,38 +692,40 @@
       </c>
       <c r="L5"/>
       <c r="M5" t="n">
-        <v>25</v>
-      </c>
-      <c r="N5"/>
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>69</v>
+      </c>
       <c r="O5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4165</v>
+        <v>3279</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" t="n">
-        <v>2071109</v>
+        <v>2071090</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J6"/>
       <c r="K6" t="b">
@@ -663,38 +733,38 @@
       </c>
       <c r="L6"/>
       <c r="M6" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N6"/>
       <c r="O6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1700</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.395833333333333</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" t="n">
-        <v>2107120</v>
+        <v>2071257</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J7"/>
       <c r="K7" t="b">
@@ -702,38 +772,38 @@
       </c>
       <c r="L7"/>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N7"/>
-      <c r="O7" t="n">
-        <v>547906067</v>
+      <c r="O7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2959</v>
+        <v>3453</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.395833333333333</v>
+        <v>0.375</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" t="n">
-        <v>7220184</v>
+        <v>2071040</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="b">
@@ -741,40 +811,38 @@
       </c>
       <c r="L8"/>
       <c r="M8" t="n">
-        <v>10</v>
-      </c>
-      <c r="N8" t="s">
-        <v>56</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N8"/>
       <c r="O8" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3084</v>
+        <v>6685</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>0.375</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" t="n">
-        <v>1321322</v>
+        <v>8250465</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J9"/>
       <c r="K9" t="b">
@@ -785,37 +853,34 @@
         <v>10</v>
       </c>
       <c r="N9" t="s">
-        <v>56</v>
-      </c>
-      <c r="O9" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7152</v>
+        <v>4203</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" t="n">
-        <v>2145090</v>
+        <v>1008072</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J10"/>
       <c r="K10" t="b">
@@ -823,40 +888,38 @@
       </c>
       <c r="L10"/>
       <c r="M10" t="n">
-        <v>10</v>
-      </c>
-      <c r="N10" t="s">
-        <v>56</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N10"/>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1465</v>
+        <v>4120</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" t="n">
-        <v>2071190</v>
+        <v>2300229</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J11"/>
       <c r="K11" t="b">
@@ -864,13 +927,11 @@
       </c>
       <c r="L11"/>
       <c r="M11" t="n">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>56</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N11"/>
       <c r="O11" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
@@ -881,10 +942,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>0.395833333333333</v>
@@ -897,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="b">
@@ -909,34 +970,34 @@
       </c>
       <c r="N12"/>
       <c r="O12" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1751</v>
+        <v>822</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" t="n">
-        <v>8222222</v>
+        <v>2071070</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J13"/>
       <c r="K13" t="b">
@@ -948,34 +1009,34 @@
       </c>
       <c r="N13"/>
       <c r="O13" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4203</v>
+        <v>7152</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" t="n">
-        <v>1008072</v>
+        <v>2145090</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="J14"/>
       <c r="K14" t="b">
@@ -983,38 +1044,40 @@
       </c>
       <c r="L14"/>
       <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14"/>
+        <v>10</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
       <c r="O14" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6685</v>
+        <v>3084</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>0.416666666666667</v>
+        <v>0.375</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" t="n">
-        <v>8250465</v>
+        <v>1321322</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J15"/>
       <c r="K15" t="b">
@@ -1025,34 +1088,37 @@
         <v>10</v>
       </c>
       <c r="N15" t="s">
-        <v>56</v>
+        <v>69</v>
+      </c>
+      <c r="O15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4120</v>
+        <v>2959</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>0.375</v>
+        <v>0.395833333333333</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" t="n">
-        <v>2300229</v>
+        <v>7220184</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J16"/>
       <c r="K16" t="b">
@@ -1060,38 +1126,40 @@
       </c>
       <c r="L16"/>
       <c r="M16" t="n">
-        <v>25</v>
-      </c>
-      <c r="N16"/>
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>69</v>
+      </c>
       <c r="O16" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>822</v>
+        <v>1700</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>0.375</v>
+        <v>0.395833333333333</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" t="n">
-        <v>2071070</v>
+        <v>2107120</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J17"/>
       <c r="K17" t="b">
@@ -1099,38 +1167,38 @@
       </c>
       <c r="L17"/>
       <c r="M17" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N17"/>
-      <c r="O17" t="s">
-        <v>71</v>
+      <c r="O17" t="n">
+        <v>547906067</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>274</v>
+        <v>4165</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" t="n">
-        <v>2071083</v>
+        <v>2071109</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J18"/>
       <c r="K18" t="b">
@@ -1142,34 +1210,34 @@
       </c>
       <c r="N18"/>
       <c r="O18" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7138</v>
+        <v>2599</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>0.375</v>
+        <v>0.395833333333333</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" t="n">
-        <v>7150479</v>
+        <v>230740</v>
       </c>
       <c r="H19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J19"/>
       <c r="K19" t="b">
@@ -1177,153 +1245,153 @@
       </c>
       <c r="L19"/>
       <c r="M19" t="n">
-        <v>10</v>
-      </c>
-      <c r="N19" t="s">
-        <v>56</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N19"/>
       <c r="O19" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>214954968</v>
+        <v>3734</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20"/>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>2071186</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J20"/>
       <c r="K20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20"/>
       <c r="M20" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="N20"/>
-      <c r="O20" t="n">
-        <v>523863228</v>
+      <c r="O20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6885</v>
+        <v>2029</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>2071030</v>
       </c>
       <c r="H21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J21"/>
       <c r="K21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21"/>
       <c r="M21" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="N21"/>
       <c r="O21" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>29614112</v>
+        <v>1751</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C22"/>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>8222222</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J22"/>
       <c r="K22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22"/>
       <c r="M22" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="N22"/>
-      <c r="O22" t="n">
-        <v>523863228</v>
+      <c r="O22" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3453</v>
+        <v>27931617</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
+      <c r="C23"/>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" t="n">
-        <v>2071040</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J23"/>
       <c r="K23" t="b">
@@ -1331,38 +1399,38 @@
       </c>
       <c r="L23"/>
       <c r="M23" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="N23"/>
-      <c r="O23" t="s">
-        <v>75</v>
+      <c r="O23" t="n">
+        <v>543348646</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4377</v>
+        <v>883</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>0.375</v>
+        <v>0.416666666666667</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" t="n">
-        <v>2068536</v>
+        <v>2083331</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J24"/>
       <c r="K24" t="b">
@@ -1370,38 +1438,38 @@
       </c>
       <c r="L24"/>
       <c r="M24" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N24"/>
       <c r="O24" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>7</v>
+        <v>5178</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>0.395833333333333</v>
+        <v>0.375</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" t="n">
-        <v>2071257</v>
+        <v>2071131</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J25"/>
       <c r="K25" t="b">
@@ -1413,34 +1481,34 @@
       </c>
       <c r="N25"/>
       <c r="O25" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4828</v>
+        <v>5723</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" t="n">
-        <v>2800900</v>
+        <v>1202015</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J26"/>
       <c r="K26" t="b">
@@ -1448,38 +1516,38 @@
       </c>
       <c r="L26"/>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N26"/>
       <c r="O26" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3613</v>
+        <v>5179</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" t="n">
-        <v>9471203</v>
+        <v>2071119</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="J27"/>
       <c r="K27" t="b">
@@ -1487,40 +1555,38 @@
       </c>
       <c r="L27"/>
       <c r="M27" t="n">
-        <v>10</v>
-      </c>
-      <c r="N27" t="s">
-        <v>56</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N27"/>
       <c r="O27" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>6283</v>
+        <v>2011</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" t="n">
-        <v>2071517</v>
+        <v>2071154</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J28"/>
       <c r="K28" t="b">
@@ -1531,35 +1597,35 @@
         <v>25</v>
       </c>
       <c r="N28"/>
-      <c r="O28" t="s">
-        <v>80</v>
+      <c r="O28" t="n">
+        <v>544710406</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>603</v>
+        <v>4008</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" t="n">
-        <v>2071005</v>
+        <v>2071003</v>
       </c>
       <c r="H29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="J29"/>
       <c r="K29" t="b">
@@ -1567,38 +1633,38 @@
       </c>
       <c r="L29"/>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N29"/>
       <c r="O29" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>7207</v>
+        <v>4007</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>2071058</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="J30"/>
       <c r="K30" t="b">
@@ -1606,40 +1672,38 @@
       </c>
       <c r="L30"/>
       <c r="M30" t="n">
-        <v>10</v>
-      </c>
-      <c r="N30" t="s">
-        <v>56</v>
-      </c>
-      <c r="O30" t="s">
-        <v>82</v>
+        <v>25</v>
+      </c>
+      <c r="N30"/>
+      <c r="O30" t="n">
+        <v>542206373</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>273</v>
+        <v>4006</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" t="n">
-        <v>2071039</v>
+        <v>2071046</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J31"/>
       <c r="K31" t="b">
@@ -1651,32 +1715,34 @@
       </c>
       <c r="N31"/>
       <c r="O31" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>57967960</v>
+        <v>3613</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
-      <c r="C32"/>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>0.375</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>9471203</v>
       </c>
       <c r="H32" t="b">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J32"/>
       <c r="K32" t="b">
@@ -1684,11 +1750,477 @@
       </c>
       <c r="L32"/>
       <c r="M32" t="n">
+        <v>10</v>
+      </c>
+      <c r="N32" t="s">
+        <v>69</v>
+      </c>
+      <c r="O32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1755</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" t="n">
+        <v>2071017</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
+      </c>
+      <c r="J33"/>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33"/>
+      <c r="M33" t="n">
+        <v>25</v>
+      </c>
+      <c r="N33"/>
+      <c r="O33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4828</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" t="n">
+        <v>2800900</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34"/>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34"/>
+      <c r="O34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>273</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" t="n">
+        <v>2071039</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>62</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35"/>
+      <c r="M35" t="n">
+        <v>25</v>
+      </c>
+      <c r="N35"/>
+      <c r="O35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>274</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" t="n">
+        <v>2071083</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36"/>
+      <c r="M36" t="n">
+        <v>25</v>
+      </c>
+      <c r="N36"/>
+      <c r="O36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>7138</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" t="n">
+        <v>7150479</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37"/>
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37"/>
+      <c r="M37" t="n">
+        <v>10</v>
+      </c>
+      <c r="N37" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>214954968</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38"/>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38"/>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38"/>
+      <c r="M38" t="n">
+        <v>50</v>
+      </c>
+      <c r="N38"/>
+      <c r="O38" t="n">
+        <v>523863228</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>6885</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39"/>
+      <c r="M39" t="n">
+        <v>35</v>
+      </c>
+      <c r="N39"/>
+      <c r="O39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>29614112</v>
+      </c>
+      <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="N32"/>
-      <c r="O32" t="n">
+      <c r="C40"/>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>62</v>
+      </c>
+      <c r="J40"/>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40"/>
+      <c r="M40" t="n">
+        <v>50</v>
+      </c>
+      <c r="N40"/>
+      <c r="O40" t="n">
+        <v>523863228</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>57967960</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>62</v>
+      </c>
+      <c r="J41"/>
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41"/>
+      <c r="M41" t="n">
+        <v>40</v>
+      </c>
+      <c r="N41"/>
+      <c r="O41" t="n">
         <v>584731700</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4377</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" t="n">
+        <v>2068536</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>62</v>
+      </c>
+      <c r="J42"/>
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42"/>
+      <c r="M42" t="n">
+        <v>25</v>
+      </c>
+      <c r="N42"/>
+      <c r="O42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>5862</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" t="n">
+        <v>2071601</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43"/>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43" t="n">
+        <v>25</v>
+      </c>
+      <c r="N43"/>
+      <c r="O43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4891</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" t="n">
+        <v>2071179</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44"/>
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44"/>
+      <c r="M44" t="n">
+        <v>25</v>
+      </c>
+      <c r="N44"/>
+      <c r="O44" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>